<commit_message>
new dod preprocess outputs, parser and util updates
</commit_message>
<xml_diff>
--- a/docs/DOD/AV45_BL_means_Dec2014_99.xlsx
+++ b/docs/DOD/AV45_BL_means_Dec2014_99.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25540" yWindow="-80" windowWidth="25600" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="47200" windowHeight="26580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AV45_BL_means_02-Dec-2014_99.cs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -144,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SCRNO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ADAS_TOTSCORE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -217,11 +213,21 @@
     <t>CSF_ptau</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>PID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -607,7 +613,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -634,10 +640,10 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -658,34 +664,34 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
       <c r="O1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q1" t="s">
         <v>35</v>
       </c>
       <c r="R1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>10</v>
@@ -697,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="V1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W1" t="s">
         <v>3</v>
@@ -742,31 +748,31 @@
         <v>19</v>
       </c>
       <c r="AK1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" t="s">
         <v>46</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>47</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>49</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>52</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>53</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -11403,7 +11409,7 @@
         <v>63832</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -40558,6 +40564,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="E3:E1048576"/>
   </sortState>

</xml_diff>